<commit_message>
PnL and account equity working
</commit_message>
<xml_diff>
--- a/Week-9-project/export.xlsx
+++ b/Week-9-project/export.xlsx
@@ -1269,7 +1269,7 @@
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O19" t="n">
@@ -1410,7 +1410,7 @@
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O22" t="n">
@@ -1551,7 +1551,7 @@
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O25" t="n">
@@ -2122,7 +2122,7 @@
       <c r="M38" t="inlineStr"/>
       <c r="N38" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O38" t="n">
@@ -2392,7 +2392,7 @@
       <c r="M44" t="inlineStr"/>
       <c r="N44" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O44" t="n">
@@ -2705,7 +2705,7 @@
       <c r="M51" t="inlineStr"/>
       <c r="N51" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O51" t="n">
@@ -3534,7 +3534,7 @@
       <c r="M70" t="inlineStr"/>
       <c r="N70" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O70" t="n">
@@ -3718,7 +3718,7 @@
       <c r="M74" t="inlineStr"/>
       <c r="N74" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O74" t="n">
@@ -4504,7 +4504,7 @@
       <c r="M92" t="inlineStr"/>
       <c r="N92" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O92" t="n">
@@ -4817,7 +4817,7 @@
       <c r="M99" t="inlineStr"/>
       <c r="N99" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O99" t="n">
@@ -4958,7 +4958,7 @@
       <c r="M102" t="inlineStr"/>
       <c r="N102" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O102" t="n">
@@ -5658,7 +5658,7 @@
       <c r="M118" t="inlineStr"/>
       <c r="N118" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O118" t="n">
@@ -6186,7 +6186,7 @@
       <c r="M130" t="inlineStr"/>
       <c r="N130" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O130" t="n">
@@ -6284,7 +6284,7 @@
       <c r="M132" t="inlineStr"/>
       <c r="N132" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O132" t="n">
@@ -7156,7 +7156,7 @@
       <c r="M152" t="inlineStr"/>
       <c r="N152" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O152" t="n">
@@ -7297,7 +7297,7 @@
       <c r="M155" t="inlineStr"/>
       <c r="N155" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O155" t="n">
@@ -7438,7 +7438,7 @@
       <c r="M158" t="inlineStr"/>
       <c r="N158" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O158" t="n">
@@ -7622,7 +7622,7 @@
       <c r="M162" t="inlineStr"/>
       <c r="N162" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O162" t="n">
@@ -7720,7 +7720,7 @@
       <c r="M164" t="inlineStr"/>
       <c r="N164" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O164" t="n">
@@ -8205,7 +8205,7 @@
       <c r="M175" t="inlineStr"/>
       <c r="N175" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O175" t="n">
@@ -8303,7 +8303,7 @@
       <c r="M177" t="inlineStr"/>
       <c r="N177" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O177" t="n">
@@ -8487,7 +8487,7 @@
       <c r="M181" t="inlineStr"/>
       <c r="N181" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O181" t="n">
@@ -8671,7 +8671,7 @@
       <c r="M185" t="inlineStr"/>
       <c r="N185" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O185" t="n">
@@ -9027,7 +9027,7 @@
       <c r="M193" t="inlineStr"/>
       <c r="N193" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O193" t="n">
@@ -9125,7 +9125,7 @@
       <c r="M195" t="inlineStr"/>
       <c r="N195" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O195" t="n">
@@ -9223,7 +9223,7 @@
       <c r="M197" t="inlineStr"/>
       <c r="N197" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O197" t="n">
@@ -9708,7 +9708,7 @@
       <c r="M208" t="inlineStr"/>
       <c r="N208" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O208" t="n">
@@ -9806,7 +9806,7 @@
       <c r="M210" t="inlineStr"/>
       <c r="N210" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O210" t="n">
@@ -10076,7 +10076,7 @@
       <c r="M216" t="inlineStr"/>
       <c r="N216" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O216" t="n">
@@ -10260,7 +10260,7 @@
       <c r="M220" t="inlineStr"/>
       <c r="N220" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O220" t="n">
@@ -10444,7 +10444,7 @@
       <c r="M224" t="inlineStr"/>
       <c r="N224" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O224" t="n">
@@ -10542,7 +10542,7 @@
       <c r="M226" t="inlineStr"/>
       <c r="N226" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O226" t="n">
@@ -10726,7 +10726,7 @@
       <c r="M230" t="inlineStr"/>
       <c r="N230" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O230" t="n">
@@ -10953,7 +10953,7 @@
       <c r="M235" t="inlineStr"/>
       <c r="N235" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O235" t="n">
@@ -11137,7 +11137,7 @@
       <c r="M239" t="inlineStr"/>
       <c r="N239" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O239" t="n">
@@ -11407,7 +11407,7 @@
       <c r="M245" t="inlineStr"/>
       <c r="N245" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O245" t="n">
@@ -11935,7 +11935,7 @@
       <c r="M257" t="inlineStr"/>
       <c r="N257" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O257" t="n">
@@ -12162,7 +12162,7 @@
       <c r="M262" t="inlineStr"/>
       <c r="N262" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O262" t="n">
@@ -12346,7 +12346,7 @@
       <c r="M266" t="inlineStr"/>
       <c r="N266" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O266" t="n">
@@ -12444,7 +12444,7 @@
       <c r="M268" t="inlineStr"/>
       <c r="N268" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O268" t="n">
@@ -12542,7 +12542,7 @@
       <c r="M270" t="inlineStr"/>
       <c r="N270" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O270" t="n">
@@ -12769,7 +12769,7 @@
       <c r="M275" t="inlineStr"/>
       <c r="N275" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O275" t="n">
@@ -13125,7 +13125,7 @@
       <c r="M283" t="inlineStr"/>
       <c r="N283" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O283" t="n">
@@ -13223,7 +13223,7 @@
       <c r="M285" t="inlineStr"/>
       <c r="N285" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O285" t="n">
@@ -13407,7 +13407,7 @@
       <c r="M289" t="inlineStr"/>
       <c r="N289" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O289" t="n">
@@ -13720,7 +13720,7 @@
       <c r="M296" t="inlineStr"/>
       <c r="N296" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O296" t="n">
@@ -13861,7 +13861,7 @@
       <c r="M299" t="inlineStr"/>
       <c r="N299" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O299" t="n">
@@ -13959,7 +13959,7 @@
       <c r="M301" t="inlineStr"/>
       <c r="N301" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O301" t="n">
@@ -14315,7 +14315,7 @@
       <c r="M309" t="inlineStr"/>
       <c r="N309" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O309" t="n">
@@ -14972,7 +14972,7 @@
       <c r="M324" t="inlineStr"/>
       <c r="N324" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O324" t="n">
@@ -15113,7 +15113,7 @@
       <c r="M327" t="inlineStr"/>
       <c r="N327" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O327" t="n">
@@ -15727,7 +15727,7 @@
       <c r="M341" t="inlineStr"/>
       <c r="N341" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O341" t="n">
@@ -15911,7 +15911,7 @@
       <c r="M345" t="inlineStr"/>
       <c r="N345" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O345" t="n">
@@ -16439,7 +16439,7 @@
       <c r="M357" t="inlineStr"/>
       <c r="N357" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O357" t="n">
@@ -17010,7 +17010,7 @@
       <c r="M370" t="inlineStr"/>
       <c r="N370" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O370" t="n">
@@ -17108,7 +17108,7 @@
       <c r="M372" t="inlineStr"/>
       <c r="N372" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O372" t="n">
@@ -17249,7 +17249,7 @@
       <c r="M375" t="inlineStr"/>
       <c r="N375" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O375" t="n">
@@ -17476,7 +17476,7 @@
       <c r="M380" t="inlineStr"/>
       <c r="N380" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O380" t="n">
@@ -17875,7 +17875,7 @@
       <c r="M389" t="inlineStr"/>
       <c r="N389" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O389" t="n">
@@ -18016,7 +18016,7 @@
       <c r="M392" t="inlineStr"/>
       <c r="N392" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O392" t="n">
@@ -18114,7 +18114,7 @@
       <c r="M394" t="inlineStr"/>
       <c r="N394" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O394" t="n">
@@ -18427,7 +18427,7 @@
       <c r="M401" t="inlineStr"/>
       <c r="N401" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O401" t="n">
@@ -18912,7 +18912,7 @@
       <c r="M412" t="inlineStr"/>
       <c r="N412" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O412" t="n">
@@ -19010,7 +19010,7 @@
       <c r="M414" t="inlineStr"/>
       <c r="N414" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O414" t="n">
@@ -19280,7 +19280,7 @@
       <c r="M420" t="inlineStr"/>
       <c r="N420" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O420" t="n">
@@ -19421,7 +19421,7 @@
       <c r="M423" t="inlineStr"/>
       <c r="N423" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O423" t="n">
@@ -19648,7 +19648,7 @@
       <c r="M428" t="inlineStr"/>
       <c r="N428" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O428" t="n">
@@ -19961,7 +19961,7 @@
       <c r="M435" t="inlineStr"/>
       <c r="N435" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O435" t="n">
@@ -20876,7 +20876,7 @@
       <c r="M456" t="inlineStr"/>
       <c r="N456" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O456" t="n">
@@ -21576,7 +21576,7 @@
       <c r="M472" t="inlineStr"/>
       <c r="N472" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O472" t="n">
@@ -21846,7 +21846,7 @@
       <c r="M478" t="inlineStr"/>
       <c r="N478" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O478" t="n">
@@ -22202,7 +22202,7 @@
       <c r="M486" t="inlineStr"/>
       <c r="N486" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O486" t="n">
@@ -22816,7 +22816,7 @@
       <c r="M500" t="inlineStr"/>
       <c r="N500" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O500" t="n">
@@ -23817,7 +23817,7 @@
       <c r="M523" t="inlineStr"/>
       <c r="N523" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O523" t="n">
@@ -24173,7 +24173,7 @@
       <c r="M531" t="inlineStr"/>
       <c r="N531" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O531" t="n">
@@ -24271,7 +24271,7 @@
       <c r="M533" t="inlineStr"/>
       <c r="N533" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O533" t="n">
@@ -24369,7 +24369,7 @@
       <c r="M535" t="inlineStr"/>
       <c r="N535" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O535" t="n">
@@ -24467,7 +24467,7 @@
       <c r="M537" t="inlineStr"/>
       <c r="N537" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O537" t="n">
@@ -24909,7 +24909,7 @@
       <c r="M547" t="inlineStr"/>
       <c r="N547" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O547" t="n">
@@ -25265,7 +25265,7 @@
       <c r="M555" t="inlineStr"/>
       <c r="N555" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O555" t="n">
@@ -25836,7 +25836,7 @@
       <c r="M568" t="inlineStr"/>
       <c r="N568" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O568" t="n">
@@ -26149,7 +26149,7 @@
       <c r="M575" t="inlineStr"/>
       <c r="N575" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O575" t="n">
@@ -26763,7 +26763,7 @@
       <c r="M589" t="inlineStr"/>
       <c r="N589" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O589" t="n">
@@ -27033,7 +27033,7 @@
       <c r="M595" t="inlineStr"/>
       <c r="N595" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O595" t="n">
@@ -27174,7 +27174,7 @@
       <c r="M598" t="inlineStr"/>
       <c r="N598" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O598" t="n">
@@ -27358,7 +27358,7 @@
       <c r="M602" t="inlineStr"/>
       <c r="N602" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O602" t="n">
@@ -27456,7 +27456,7 @@
       <c r="M604" t="inlineStr"/>
       <c r="N604" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O604" t="n">
@@ -28242,7 +28242,7 @@
       <c r="M622" t="inlineStr"/>
       <c r="N622" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O622" t="n">
@@ -29544,7 +29544,7 @@
       <c r="M652" t="inlineStr"/>
       <c r="N652" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O652" t="n">
@@ -29728,7 +29728,7 @@
       <c r="M656" t="inlineStr"/>
       <c r="N656" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O656" t="n">
@@ -29869,7 +29869,7 @@
       <c r="M659" t="inlineStr"/>
       <c r="N659" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O659" t="n">
@@ -29967,7 +29967,7 @@
       <c r="M661" t="inlineStr"/>
       <c r="N661" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O661" t="n">
@@ -30280,7 +30280,7 @@
       <c r="M668" t="inlineStr"/>
       <c r="N668" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O668" t="n">
@@ -30765,7 +30765,7 @@
       <c r="M679" t="inlineStr"/>
       <c r="N679" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O679" t="n">
@@ -30863,7 +30863,7 @@
       <c r="M681" t="inlineStr"/>
       <c r="N681" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O681" t="n">
@@ -31090,7 +31090,7 @@
       <c r="M686" t="inlineStr"/>
       <c r="N686" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O686" t="n">
@@ -31360,7 +31360,7 @@
       <c r="M692" t="inlineStr"/>
       <c r="N692" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O692" t="n">
@@ -31458,7 +31458,7 @@
       <c r="M694" t="inlineStr"/>
       <c r="N694" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O694" t="n">
@@ -31599,7 +31599,7 @@
       <c r="M697" t="inlineStr"/>
       <c r="N697" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O697" t="n">
@@ -32041,7 +32041,7 @@
       <c r="M707" t="inlineStr"/>
       <c r="N707" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O707" t="n">
@@ -32225,7 +32225,7 @@
       <c r="M711" t="inlineStr"/>
       <c r="N711" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O711" t="n">
@@ -33097,7 +33097,7 @@
       <c r="M731" t="inlineStr"/>
       <c r="N731" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O731" t="n">
@@ -33367,7 +33367,7 @@
       <c r="M737" t="inlineStr"/>
       <c r="N737" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O737" t="n">
@@ -33594,7 +33594,7 @@
       <c r="M742" t="inlineStr"/>
       <c r="N742" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O742" t="n">
@@ -33778,7 +33778,7 @@
       <c r="M746" t="inlineStr"/>
       <c r="N746" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O746" t="n">
@@ -34091,7 +34091,7 @@
       <c r="M753" t="inlineStr"/>
       <c r="N753" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O753" t="n">
@@ -34232,7 +34232,7 @@
       <c r="M756" t="inlineStr"/>
       <c r="N756" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O756" t="n">
@@ -34674,7 +34674,7 @@
       <c r="M766" t="inlineStr"/>
       <c r="N766" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O766" t="n">
@@ -35202,7 +35202,7 @@
       <c r="M778" t="inlineStr"/>
       <c r="N778" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O778" t="n">
@@ -35386,7 +35386,7 @@
       <c r="M782" t="inlineStr"/>
       <c r="N782" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O782" t="n">
@@ -35484,7 +35484,7 @@
       <c r="M784" t="inlineStr"/>
       <c r="N784" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O784" t="n">
@@ -35625,7 +35625,7 @@
       <c r="M787" t="inlineStr"/>
       <c r="N787" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O787" t="n">
@@ -35723,7 +35723,7 @@
       <c r="M789" t="inlineStr"/>
       <c r="N789" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O789" t="n">
@@ -35821,7 +35821,7 @@
       <c r="M791" t="inlineStr"/>
       <c r="N791" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O791" t="n">
@@ -36607,7 +36607,7 @@
       <c r="M809" t="inlineStr"/>
       <c r="N809" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O809" t="n">
@@ -36963,7 +36963,7 @@
       <c r="M817" t="inlineStr"/>
       <c r="N817" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O817" t="n">
@@ -37147,7 +37147,7 @@
       <c r="M821" t="inlineStr"/>
       <c r="N821" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O821" t="n">
@@ -37632,7 +37632,7 @@
       <c r="M832" t="inlineStr"/>
       <c r="N832" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O832" t="n">
@@ -37730,7 +37730,7 @@
       <c r="M834" t="inlineStr"/>
       <c r="N834" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O834" t="n">
@@ -37914,7 +37914,7 @@
       <c r="M838" t="inlineStr"/>
       <c r="N838" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O838" t="n">
@@ -38141,7 +38141,7 @@
       <c r="M843" t="inlineStr"/>
       <c r="N843" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O843" t="n">
@@ -38497,7 +38497,7 @@
       <c r="M851" t="inlineStr"/>
       <c r="N851" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O851" t="n">
@@ -38810,7 +38810,7 @@
       <c r="M858" t="inlineStr"/>
       <c r="N858" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O858" t="n">
@@ -39166,7 +39166,7 @@
       <c r="M866" t="inlineStr"/>
       <c r="N866" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O866" t="n">
@@ -39307,7 +39307,7 @@
       <c r="M869" t="inlineStr"/>
       <c r="N869" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O869" t="n">
@@ -39620,7 +39620,7 @@
       <c r="M876" t="inlineStr"/>
       <c r="N876" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O876" t="n">
@@ -40019,7 +40019,7 @@
       <c r="M885" t="inlineStr"/>
       <c r="N885" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O885" t="n">
@@ -40246,7 +40246,7 @@
       <c r="M890" t="inlineStr"/>
       <c r="N890" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O890" t="n">
@@ -40473,7 +40473,7 @@
       <c r="M895" t="inlineStr"/>
       <c r="N895" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O895" t="n">
@@ -41259,7 +41259,7 @@
       <c r="M913" t="inlineStr"/>
       <c r="N913" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O913" t="n">
@@ -41529,7 +41529,7 @@
       <c r="M919" t="inlineStr"/>
       <c r="N919" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O919" t="n">
@@ -41670,7 +41670,7 @@
       <c r="M922" t="inlineStr"/>
       <c r="N922" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O922" t="n">
@@ -41983,7 +41983,7 @@
       <c r="M929" t="inlineStr"/>
       <c r="N929" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O929" t="n">
@@ -42253,7 +42253,7 @@
       <c r="M935" t="inlineStr"/>
       <c r="N935" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O935" t="n">
@@ -42652,7 +42652,7 @@
       <c r="M944" t="inlineStr"/>
       <c r="N944" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O944" t="n">
@@ -43223,7 +43223,7 @@
       <c r="M957" t="inlineStr"/>
       <c r="N957" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O957" t="n">
@@ -43321,7 +43321,7 @@
       <c r="M959" t="inlineStr"/>
       <c r="N959" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O959" t="n">
@@ -43419,7 +43419,7 @@
       <c r="M961" t="inlineStr"/>
       <c r="N961" t="inlineStr">
         <is>
-          <t>exit short</t>
+          <t>exit_short</t>
         </is>
       </c>
       <c r="O961" t="n">
@@ -44850,7 +44850,7 @@
       <c r="M994" t="inlineStr"/>
       <c r="N994" t="inlineStr">
         <is>
-          <t>exit long</t>
+          <t>exit_long</t>
         </is>
       </c>
       <c r="O994" t="n">

</xml_diff>